<commit_message>
Job queries coded, console removed, multiple option coded
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/4173/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/4173/Actual/JobMaterial.xlsx
@@ -47,43 +47,43 @@
     <t>Ink / Varnish</t>
   </si>
   <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>WF Print F 4x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyan - Wide Format UV - </t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>DF394 - Digital Ink/AC (Default, Lbs)</t>
+  </si>
+  <si>
+    <t>ISM Dallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black - Wide Format UV - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magenta - Wide Format UV - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow - Wide Format UV - </t>
+  </si>
+  <si>
     <t>Flat  2p</t>
   </si>
   <si>
-    <t>WF Print F 4x0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellow - Wide Format UV - </t>
-  </si>
-  <si>
     <t>0.07</t>
-  </si>
-  <si>
-    <t>lbs</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>DF394 - Digital Ink/AC (Default, Lbs)</t>
-  </si>
-  <si>
-    <t>ISM Dallas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magenta - Wide Format UV - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black - Wide Format UV - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyan - Wide Format UV - </t>
-  </si>
-  <si>
-    <t>Banner</t>
-  </si>
-  <si>
-    <t>0.08</t>
   </si>
   <si>
     <t>Sheet</t>
@@ -944,7 +944,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s" s="45">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s" s="46">
         <v>23</v>
@@ -976,7 +976,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="s" s="55">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s" s="56">
         <v>23</v>
@@ -1008,7 +1008,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s" s="65">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s" s="66">
         <v>23</v>
@@ -1040,7 +1040,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="s" s="75">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s" s="76">
         <v>23</v>
@@ -1066,7 +1066,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s" s="83">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s" s="84">
         <v>25</v>
@@ -1098,7 +1098,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s" s="93">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s" s="94">
         <v>25</v>

</xml_diff>